<commit_message>
Make changes to excel file for consistency
</commit_message>
<xml_diff>
--- a/flow.xlsx
+++ b/flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thakk\Documents\Programming\pandas-to-postgres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F730F-CBA1-4DF5-BB44-7B2EF7DEF1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C579A8-BA61-4F06-8DD0-259E306833F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8E236BDD-DEAE-415C-83E6-B0048DC40BBF}"/>
   </bookViews>
@@ -158,15 +158,6 @@
     <t>Austin, TX</t>
   </si>
   <si>
-    <t>patientID</t>
-  </si>
-  <si>
-    <t>first name</t>
-  </si>
-  <si>
-    <t>last name</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -174,6 +165,15 @@
   </si>
   <si>
     <t>dob</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>patientid</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,22 +564,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>